<commit_message>
�️ Remove VM deployment workflow - Keep only Container Instances
</commit_message>
<xml_diff>
--- a/backend/reports_files/reporte_consolidado_2025_07.xlsx
+++ b/backend/reports_files/reporte_consolidado_2025_07.xlsx
@@ -513,7 +513,7 @@
     <row r="4" ht="18" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Generado: 12/07/2025 17:16 | Total de Tickets: 146</t>
+          <t>Generado: 13/07/2025 08:06 | Total de Tickets: 146</t>
         </is>
       </c>
     </row>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="K14" s="6" t="inlineStr">
         <is>
-          <t>ticket resuelto</t>
+          <t>resuelto</t>
         </is>
       </c>
     </row>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="K15" s="6" t="inlineStr">
         <is>
-          <t>resuelto</t>
+          <t>ticket resuelto</t>
         </is>
       </c>
     </row>
@@ -2473,7 +2473,7 @@
       </c>
       <c r="D40" s="5" t="inlineStr">
         <is>
-          <t>asignado</t>
+          <t>cerrado</t>
         </is>
       </c>
       <c r="E40" s="5" t="inlineStr">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="G40" s="6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>12/07/2025 23:18</t>
         </is>
       </c>
       <c r="H40" s="6" t="inlineStr">
@@ -2503,12 +2503,12 @@
       </c>
       <c r="J40" s="6" t="inlineStr">
         <is>
-          <t>Sin fecha</t>
+          <t>12/07/2025 23:18</t>
         </is>
       </c>
       <c r="K40" s="6" t="inlineStr">
         <is>
-          <t>Sin resolución</t>
+          <t>TEST RESOLUTION NOTES for TKT-000106 - This should appear in email notifications</t>
         </is>
       </c>
     </row>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="K41" s="6" t="inlineStr">
         <is>
-          <t>ticket resuelto</t>
+          <t>resolucion 2</t>
         </is>
       </c>
     </row>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="K42" s="6" t="inlineStr">
         <is>
-          <t>resolucion 2</t>
+          <t>ticket resuelto</t>
         </is>
       </c>
     </row>
@@ -4525,7 +4525,7 @@
       </c>
       <c r="D76" s="5" t="inlineStr">
         <is>
-          <t>nuevo</t>
+          <t>cerrado</t>
         </is>
       </c>
       <c r="E76" s="5" t="inlineStr">
@@ -4540,7 +4540,7 @@
       </c>
       <c r="G76" s="6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>12/07/2025 23:19</t>
         </is>
       </c>
       <c r="H76" s="6" t="inlineStr">
@@ -4555,12 +4555,12 @@
       </c>
       <c r="J76" s="6" t="inlineStr">
         <is>
-          <t>Sin fecha</t>
+          <t>12/07/2025 23:19</t>
         </is>
       </c>
       <c r="K76" s="6" t="inlineStr">
         <is>
-          <t>Sin resolución</t>
+          <t>prueba de que si se resolvvio ticket 65</t>
         </is>
       </c>
     </row>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="D77" s="5" t="inlineStr">
         <is>
-          <t>nuevo</t>
+          <t>cerrado</t>
         </is>
       </c>
       <c r="E77" s="5" t="inlineStr">
@@ -4597,7 +4597,7 @@
       </c>
       <c r="G77" s="6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>12/07/2025 23:27</t>
         </is>
       </c>
       <c r="H77" s="6" t="inlineStr">
@@ -4612,12 +4612,12 @@
       </c>
       <c r="J77" s="6" t="inlineStr">
         <is>
-          <t>Sin fecha</t>
+          <t>12/07/2025 23:27</t>
         </is>
       </c>
       <c r="K77" s="6" t="inlineStr">
         <is>
-          <t>Sin resolución</t>
+          <t>resolucion ticket 64</t>
         </is>
       </c>
     </row>
@@ -8436,7 +8436,7 @@
       </c>
       <c r="K144" s="6" t="inlineStr">
         <is>
-          <t>sdsds</t>
+          <t>34343434</t>
         </is>
       </c>
     </row>
@@ -8493,7 +8493,7 @@
       </c>
       <c r="K145" s="6" t="inlineStr">
         <is>
-          <t>34343434</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -8550,7 +8550,7 @@
       </c>
       <c r="K146" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>prueba de resolucion 40</t>
         </is>
       </c>
     </row>
@@ -8607,7 +8607,7 @@
       </c>
       <c r="K147" s="6" t="inlineStr">
         <is>
-          <t>prueba de resolucion 40</t>
+          <t>sdsds</t>
         </is>
       </c>
     </row>

</xml_diff>